<commit_message>
t tests and updated results
</commit_message>
<xml_diff>
--- a/parameter_files/test/de_dg_gw_lower.xlsx
+++ b/parameter_files/test/de_dg_gw_lower.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4efc3e9dc81381f4/Documents/SJV-gen-modeling/parameter_files/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="8_{229B6D89-0FBA-4AFF-BE65-AE5ED1F338BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51A70F0E-1E16-419D-BFB5-CD536CBA16E6}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="8_{229B6D89-0FBA-4AFF-BE65-AE5ED1F338BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36DE501E-9F96-464B-80F1-813B9FF302E4}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{47BB98F9-56B8-471D-9F66-573A44E98337}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{47BB98F9-56B8-471D-9F66-573A44E98337}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,12 +33,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Bureau of Reclamation</t>
-  </si>
-  <si>
-    <t>Legislature</t>
   </si>
   <si>
     <t>Friant Water Authority</t>
@@ -658,7 +655,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -666,13 +663,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD50E470-B89A-46FB-A183-8975EBAE0C5A}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J27" sqref="J27"/>
+      <selection pane="bottomRight" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -684,30 +681,30 @@
     <row r="1" spans="1:8" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="11" t="s">
-        <v>34</v>
-      </c>
       <c r="H1" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -718,7 +715,7 @@
     </row>
     <row r="3" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -729,7 +726,7 @@
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -740,7 +737,7 @@
     </row>
     <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -751,7 +748,7 @@
     </row>
     <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -762,7 +759,7 @@
     </row>
     <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="4">
         <v>0</v>
@@ -775,7 +772,7 @@
     </row>
     <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -786,7 +783,7 @@
     </row>
     <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -797,7 +794,7 @@
     </row>
     <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -856,8 +853,8 @@
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="3" t="s">
-        <v>5</v>
+      <c r="A16" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -881,7 +878,9 @@
       <c r="A18" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="4"/>
+      <c r="B18" s="4">
+        <v>0.5</v>
+      </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -892,9 +891,7 @@
       <c r="A19" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="4">
-        <v>0.5</v>
-      </c>
+      <c r="B19" s="5"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
@@ -902,44 +899,46 @@
       <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
+      <c r="A20" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20">
+        <v>-0.2</v>
+      </c>
+      <c r="D20">
+        <v>-0.2</v>
+      </c>
+      <c r="E20">
+        <v>-0.2</v>
+      </c>
+      <c r="F20">
+        <v>-0.2</v>
+      </c>
+      <c r="G20">
+        <v>-0.2</v>
+      </c>
+      <c r="H20">
+        <v>-0.2</v>
+      </c>
     </row>
     <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21">
-        <v>-0.5</v>
-      </c>
-      <c r="D21">
-        <v>-0.5</v>
-      </c>
-      <c r="E21">
-        <v>-0.5</v>
-      </c>
-      <c r="F21">
-        <v>-0.5</v>
-      </c>
-      <c r="G21">
-        <v>-0.2</v>
-      </c>
-      <c r="H21">
-        <v>-0.2</v>
-      </c>
+      <c r="A21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="4"/>
+      <c r="B22" s="5">
+        <v>0</v>
+      </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
@@ -951,7 +950,7 @@
         <v>7</v>
       </c>
       <c r="B23" s="5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -963,9 +962,7 @@
       <c r="A24" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="5">
-        <v>0.5</v>
-      </c>
+      <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
@@ -995,7 +992,7 @@
       <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B27" s="4"/>
@@ -1016,8 +1013,8 @@
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="6" t="s">
+    <row r="29" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B29" s="4"/>
@@ -1027,19 +1024,8 @@
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" s="12"/>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>